<commit_message>
Excel for Building formulas in sql
</commit_message>
<xml_diff>
--- a/excel for assigment 2.xlsx
+++ b/excel for assigment 2.xlsx
@@ -446,11 +446,11 @@
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" t="str">
         <f ca="1">CONCATENATE($A$1,$C$1,$D$1,$E$1,B2,$E$1,$F$1,$E$1,C2,$E$1,$F$1,D2,$G$1,$H$1)</f>
-        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Mark','Dunkirk ',1);</v>
+        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Mark','Dunkirk ',2);</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -462,11 +462,11 @@
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D31" ca="1" si="0">RANDBETWEEN(1,5)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E31" ca="1" si="1">CONCATENATE($A$1,$C$1,$D$1,$E$1,B3,$E$1,$F$1,$E$1,C3,$E$1,$F$1,D3,$G$1,$H$1)</f>
-        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Mark','Love Actually',1);</v>
+        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Mark','Love Actually',5);</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -494,11 +494,11 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Mark','Wreck It Ralph',4);</v>
+        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Mark','Wreck It Ralph',1);</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -510,11 +510,11 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Mark','Tangled',1);</v>
+        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Mark','Tangled',3);</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -526,11 +526,11 @@
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Mark','Home Alone',5);</v>
+        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Mark','Home Alone',3);</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -558,11 +558,11 @@
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Mary','Love Actually',1);</v>
+        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Mary','Love Actually',3);</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -574,11 +574,11 @@
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Mary','Die Hard',1);</v>
+        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Mary','Die Hard',4);</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -606,11 +606,11 @@
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Mary','Tangled',4);</v>
+        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Mary','Tangled',5);</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -622,11 +622,11 @@
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Mary','Home Alone',5);</v>
+        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Mary','Home Alone',4);</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -638,11 +638,11 @@
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Joseph','Dunkirk ',4);</v>
+        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Joseph','Dunkirk ',3);</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -654,11 +654,11 @@
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Joseph','Love Actually',5);</v>
+        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Joseph','Love Actually',2);</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -670,11 +670,11 @@
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Joseph','Die Hard',3);</v>
+        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Joseph','Die Hard',5);</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
@@ -686,11 +686,11 @@
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Joseph','Wreck It Ralph',5);</v>
+        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Joseph','Wreck It Ralph',4);</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
@@ -702,11 +702,11 @@
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Joseph','Tangled',1);</v>
+        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Joseph','Tangled',5);</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
@@ -750,11 +750,11 @@
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Paul','Love Actually',1);</v>
+        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Paul','Love Actually',2);</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
@@ -766,11 +766,11 @@
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Paul','Die Hard',3);</v>
+        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Paul','Die Hard',2);</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
@@ -782,11 +782,11 @@
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Paul','Wreck It Ralph',3);</v>
+        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Paul','Wreck It Ralph',4);</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
@@ -798,11 +798,11 @@
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Paul','Tangled',3);</v>
+        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Paul','Tangled',4);</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
@@ -814,11 +814,11 @@
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Paul','Home Alone',5);</v>
+        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Paul','Home Alone',4);</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
@@ -830,11 +830,11 @@
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Luke','Dunkirk ',2);</v>
+        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Luke','Dunkirk ',4);</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
@@ -846,11 +846,11 @@
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E27" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Luke','Love Actually',4);</v>
+        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Luke','Love Actually',1);</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
@@ -862,11 +862,11 @@
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Luke','Die Hard',5);</v>
+        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Luke','Die Hard',3);</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
@@ -878,11 +878,11 @@
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E29" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Luke','Wreck It Ralph',4);</v>
+        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Luke','Wreck It Ralph',2);</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.2">
@@ -894,11 +894,11 @@
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Luke','Tangled',4);</v>
+        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Luke','Tangled',5);</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.2">
@@ -910,11 +910,11 @@
       </c>
       <c r="D31">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E31" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Luke','Home Alone',4);</v>
+        <v>INSERT INTO movie_table (person, movie, rating) VALUES('Luke','Home Alone',5);</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.2">

</xml_diff>